<commit_message>
Updated inulinase tax summary tables w/ new unclassified (combined)
</commit_message>
<xml_diff>
--- a/kaiju/tax_summarized/exo.class.table.xlsx
+++ b/kaiju/tax_summarized/exo.class.table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/CRDS_Calcs/kaiju/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/Carb_CRDS/kaiju/tax_summarized/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{06C473AD-9A34-4E3C-BF56-C199A8B3B486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:40009_{06C473AD-9A34-4E3C-BF56-C199A8B3B486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{790FC5FE-E4F6-439C-8453-5519DF21345D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="12900" yWindow="105" windowWidth="15675" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="exo.class" sheetId="1" r:id="rId1"/>
@@ -20,20 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
   <si>
     <t>Spring</t>
   </si>
   <si>
-    <t>cannot be assigned to a (non-viral) class</t>
-  </si>
-  <si>
-    <t>unclassified</t>
-  </si>
-  <si>
-    <t>Viruses</t>
-  </si>
-  <si>
     <t>Summer</t>
   </si>
   <si>
@@ -52,9 +43,6 @@
     <t>42.967 ± 2.602</t>
   </si>
   <si>
-    <t>0.008 ± 0.005</t>
-  </si>
-  <si>
     <t>0.090 ± 0.025</t>
   </si>
   <si>
@@ -82,18 +70,12 @@
     <t>0.060 ± 0.056</t>
   </si>
   <si>
-    <t>6.022 ± 1.648</t>
-  </si>
-  <si>
     <t>0.122 ± 0.048</t>
   </si>
   <si>
     <t>0.004 ± 0.004</t>
   </si>
   <si>
-    <t>48.046 ± 3.366</t>
-  </si>
-  <si>
     <t>0.733 ± 0.314</t>
   </si>
   <si>
@@ -130,12 +112,6 @@
     <t>0.015 ± 0.015</t>
   </si>
   <si>
-    <t>4.446 ± 0.929</t>
-  </si>
-  <si>
-    <t>46.181 ± 2.712</t>
-  </si>
-  <si>
     <t>0.044 ± 0.016</t>
   </si>
   <si>
@@ -154,18 +130,9 @@
     <t>0.479 ± 0.208</t>
   </si>
   <si>
-    <t>0.424 ± 0.424</t>
-  </si>
-  <si>
     <t>0.008 ± 0.006</t>
   </si>
   <si>
-    <t>2.483 ± 1.583</t>
-  </si>
-  <si>
-    <t>24.026 ± 5.322</t>
-  </si>
-  <si>
     <t>Bacteria</t>
   </si>
   <si>
@@ -181,9 +148,6 @@
     <t>Bacteroidia</t>
   </si>
   <si>
-    <t>Chitinophagia</t>
-  </si>
-  <si>
     <t>Cytophagia</t>
   </si>
   <si>
@@ -211,9 +175,6 @@
     <t>Clostridia</t>
   </si>
   <si>
-    <t>Erysipelotrichia</t>
-  </si>
-  <si>
     <t>Proteobacteria</t>
   </si>
   <si>
@@ -226,12 +187,6 @@
     <t>Gammaproteobacteria</t>
   </si>
   <si>
-    <t>Verrucomicrobia</t>
-  </si>
-  <si>
-    <t>Verrucomicrobiae</t>
-  </si>
-  <si>
     <t>Eukaryota</t>
   </si>
   <si>
@@ -241,22 +196,28 @@
     <t>Eurotiomycetes</t>
   </si>
   <si>
-    <t>Chytridiomycota</t>
-  </si>
-  <si>
-    <t>Neocallimastigomycetes</t>
-  </si>
-  <si>
     <t>Domain</t>
   </si>
   <si>
     <t>Phylum</t>
+  </si>
+  <si>
+    <t>Unclassified</t>
+  </si>
+  <si>
+    <t>50.627 ± 2.190</t>
+  </si>
+  <si>
+    <t>26.939 ± 6.526</t>
+  </si>
+  <si>
+    <t>54.081 ± 1.963</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1093,11 +1054,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,19 +1073,19 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>0</v>
@@ -1132,402 +1093,282 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
         <v>27</v>
       </c>
-      <c r="E6" t="s">
-        <v>33</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
         <v>33</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
         <v>48</v>
       </c>
-      <c r="B9" t="s">
-        <v>58</v>
-      </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
         <v>48</v>
       </c>
-      <c r="B10" t="s">
-        <v>60</v>
-      </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="E15" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" t="s">
-        <v>71</v>
-      </c>
-      <c r="C18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>